<commit_message>
Update Thresholds and Results
</commit_message>
<xml_diff>
--- a/data/topics-activities/twcs-AmazonHelp-inbound-topics.xlsx
+++ b/data/topics-activities/twcs-AmazonHelp-inbound-topics.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10401"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10509"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/christophkecht/Dropbox/FIM/Master Thesis/code/electric/data/topics-activities/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/christophkecht/Dropbox/FIM/Master Thesis/code/ericsson/data/topics-activities/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8596335D-B1AA-184E-BC7A-9B9C38D5E51E}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{13573AA7-E0E6-8641-8B70-8BF4B685ABCA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-35320" yWindow="2580" windowWidth="33960" windowHeight="17080" xr2:uid="{8CB9F10C-0245-AF4C-8C1B-35237DBF815E}"/>
+    <workbookView xWindow="-35760" yWindow="740" windowWidth="33960" windowHeight="17080" xr2:uid="{8CB9F10C-0245-AF4C-8C1B-35237DBF815E}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -545,9 +545,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E6217645-8E61-C146-86DF-22EF3131DDAA}">
   <dimension ref="A1:J13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J1" sqref="J1"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
@@ -600,16 +598,16 @@
         <v>0.96</v>
       </c>
       <c r="E2">
-        <v>0.80735762223406815</v>
+        <v>0.80250335769744807</v>
       </c>
       <c r="F2">
         <v>0.9</v>
       </c>
       <c r="G2">
-        <v>0.91648351648351645</v>
+        <v>0.91648351648351656</v>
       </c>
       <c r="H2">
-        <v>0.87436410826844657</v>
+        <v>0.8717948717948717</v>
       </c>
       <c r="I2">
         <v>70</v>
@@ -728,16 +726,16 @@
         <v>0.99600000000000011</v>
       </c>
       <c r="E6">
-        <v>0.73734293731172429</v>
+        <v>0.72341598580802502</v>
       </c>
       <c r="F6">
         <v>0.95</v>
       </c>
       <c r="G6">
-        <v>0.87522522522522517</v>
+        <v>0.87816225646990409</v>
       </c>
       <c r="H6">
-        <v>0.75396825396825395</v>
+        <v>0.75000000000000011</v>
       </c>
       <c r="I6">
         <v>19</v>
@@ -792,7 +790,7 @@
         <v>0.998</v>
       </c>
       <c r="E8">
-        <v>0.8163247683778212</v>
+        <v>0.75012146732608598</v>
       </c>
       <c r="F8">
         <v>0.98499999999999999</v>
@@ -801,7 +799,7 @@
         <v>0.99234693877551017</v>
       </c>
       <c r="H8">
-        <v>0.79166666666666663</v>
+        <v>0.72727272727272729</v>
       </c>
       <c r="I8">
         <v>4</v>
@@ -824,16 +822,16 @@
         <v>0.99199999999999999</v>
       </c>
       <c r="E9">
-        <v>0.8729467923690899</v>
+        <v>0.85676283368939932</v>
       </c>
       <c r="F9">
-        <v>0.98000000000000009</v>
+        <v>0.98</v>
       </c>
       <c r="G9">
-        <v>0.98933143669985779</v>
+        <v>0.9893617021276595</v>
       </c>
       <c r="H9">
-        <v>0.86999999999999988</v>
+        <v>0.8571428571428571</v>
       </c>
       <c r="I9">
         <v>12</v>
@@ -853,19 +851,19 @@
         <v>7</v>
       </c>
       <c r="D10">
-        <v>0.98799999999999988</v>
+        <v>0.998</v>
       </c>
       <c r="E10">
-        <v>0.84882022434497251</v>
+        <v>0.7673065735892961</v>
       </c>
       <c r="F10">
-        <v>0.97499999999999998</v>
+        <v>0.98</v>
       </c>
       <c r="G10">
-        <v>0.93947368421052635</v>
+        <v>0.88365328679464805</v>
       </c>
       <c r="H10">
-        <v>0.83333333333333326</v>
+        <v>0.77777777777777779</v>
       </c>
       <c r="I10">
         <v>9</v>
@@ -917,19 +915,19 @@
         <v>28</v>
       </c>
       <c r="D12">
-        <v>0.98100000000000009</v>
+        <v>0.98000000000000009</v>
       </c>
       <c r="E12">
-        <v>0.7916632951524416</v>
+        <v>0.7376717048657514</v>
       </c>
       <c r="F12">
-        <v>0.98000000000000009</v>
+        <v>0.98</v>
       </c>
       <c r="G12">
         <v>0.98974358974358978</v>
       </c>
       <c r="H12">
-        <v>0.76666666666666661</v>
+        <v>0.7142857142857143</v>
       </c>
       <c r="I12">
         <v>5</v>
@@ -952,16 +950,16 @@
         <v>0.99700000000000011</v>
       </c>
       <c r="E13">
-        <v>0.93959648809042251</v>
+        <v>0.92343088262881712</v>
       </c>
       <c r="F13">
-        <v>0.99499999999999988</v>
+        <v>0.995</v>
       </c>
       <c r="G13">
-        <v>0.99743589743589745</v>
+        <v>0.99742268041237114</v>
       </c>
       <c r="H13">
-        <v>0.93333333333333324</v>
+        <v>0.92307692307692302</v>
       </c>
       <c r="I13">
         <v>6</v>

</xml_diff>